<commit_message>
Update CSV/XLSX with 2 additional 2022 concerts
</commit_message>
<xml_diff>
--- a/season_calendar_spreadsheets/sso_2022_season_performances.xlsx
+++ b/season_calendar_spreadsheets/sso_2022_season_performances.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sso_2022_season" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="sso_2022_season_performances" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">sso_2022_season!$A$1:$H$87</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">sso_2022_season_performances!$A$1:$H$91</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="213">
   <si>
     <t xml:space="preserve">venue</t>
   </si>
@@ -475,6 +475,24 @@
     <t xml:space="preserve">Sat 15 October</t>
   </si>
   <si>
+    <t xml:space="preserve">Sun 16 October</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sergei Prokofiev’s Peter &amp; the Wolf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many millions of young (and not so young) people have enjoyed Sergei Prokofiev’s magical musical tale of Peter, a young boy, who sets out into the deep forest to catch a wolf? Peter, his grandfather and their animal friends are brought to life by their own instrument. Peter’s bird-friend flits with the flute while his companion duck waddles along to the oboe. Lively strings hum with Peter’s cheerful energy while horns hint at the shadowy wolf at his heel. Then there’s Grandpa on the bassoon, kettle-drum hunters and even a slinking clarinet cat. Written with young ears in mind, Prokofiev’s classic is as charming and entertaining as ever.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sydneysymphony.com/concerts/prokofievs-peter-wolf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:30am</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mon 17 October</t>
   </si>
   <si>
@@ -542,6 +560,21 @@
   </si>
   <si>
     <t xml:space="preserve">Sat 29 October</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri 04 November</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lior &amp; Compassion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What happens when a great soulful voice meets the power of an orchestra? For singer-songwriter Lior and acclaimed composer Nigel Westlake, the outcome is a luminous deep-dive into the power of human compassion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sydneysymphony.com/concerts/lior-compassion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sat 05 November</t>
   </si>
   <si>
     <t xml:space="preserve">Wed 09 November</t>
@@ -640,12 +673,11 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -664,6 +696,18 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -725,11 +769,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -754,24 +798,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="0" topLeftCell="F87" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
+      <selection pane="topRight" activeCell="D93" activeCellId="0" sqref="D93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="47.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="183.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="74.99"/>
   </cols>
   <sheetData>
@@ -811,10 +854,10 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -837,10 +880,10 @@
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -863,10 +906,10 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -889,10 +932,10 @@
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -915,10 +958,10 @@
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
@@ -941,10 +984,10 @@
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="0" t="s">
@@ -967,10 +1010,10 @@
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="0" t="s">
@@ -993,10 +1036,10 @@
       <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="0" t="s">
@@ -1019,10 +1062,10 @@
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="0" t="s">
@@ -1045,10 +1088,10 @@
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="0" t="s">
@@ -1071,10 +1114,10 @@
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="0" t="s">
@@ -1097,10 +1140,10 @@
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="0" t="s">
@@ -1123,10 +1166,10 @@
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="0" t="s">
@@ -1149,10 +1192,10 @@
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="0" t="s">
@@ -1175,10 +1218,10 @@
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="D16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="0" t="s">
@@ -1201,10 +1244,10 @@
       <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="0" t="s">
@@ -1227,10 +1270,10 @@
       <c r="C18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="0" t="s">
@@ -1253,10 +1296,10 @@
       <c r="C19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="0" t="s">
@@ -1279,10 +1322,10 @@
       <c r="C20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="0" t="s">
@@ -1305,10 +1348,10 @@
       <c r="C21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="0" t="s">
@@ -1331,10 +1374,10 @@
       <c r="C22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="0" t="s">
@@ -1357,10 +1400,10 @@
       <c r="C23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="0" t="s">
@@ -1383,10 +1426,10 @@
       <c r="C24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="0" t="s">
@@ -1409,10 +1452,10 @@
       <c r="C25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="0" t="s">
@@ -1435,10 +1478,10 @@
       <c r="C26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="0" t="s">
@@ -1461,10 +1504,10 @@
       <c r="C27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="0" t="s">
@@ -1487,10 +1530,10 @@
       <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="D28" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="0" t="s">
@@ -1513,10 +1556,10 @@
       <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="D29" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="0" t="s">
@@ -1539,10 +1582,10 @@
       <c r="C30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="0" t="s">
@@ -1565,10 +1608,10 @@
       <c r="C31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="D31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="0" t="s">
@@ -1591,10 +1634,10 @@
       <c r="C32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D32" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="0" t="s">
@@ -1617,10 +1660,10 @@
       <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="D33" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="0" t="s">
@@ -1643,10 +1686,10 @@
       <c r="C34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="D34" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="0" t="s">
@@ -1669,10 +1712,10 @@
       <c r="C35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="D35" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="0" t="s">
@@ -1695,10 +1738,10 @@
       <c r="C36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F36" s="0" t="s">
@@ -1721,10 +1764,10 @@
       <c r="C37" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D37" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="0" t="s">
@@ -1747,10 +1790,10 @@
       <c r="C38" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D38" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="0" t="s">
@@ -1773,10 +1816,10 @@
       <c r="C39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F39" s="0" t="s">
@@ -1799,10 +1842,10 @@
       <c r="C40" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F40" s="0" t="s">
@@ -1825,10 +1868,10 @@
       <c r="C41" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D41" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F41" s="0" t="s">
@@ -1851,10 +1894,10 @@
       <c r="C42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="D42" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F42" s="0" t="s">
@@ -1877,10 +1920,10 @@
       <c r="C43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D43" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F43" s="0" t="s">
@@ -1903,10 +1946,10 @@
       <c r="C44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="D44" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F44" s="0" t="s">
@@ -1929,10 +1972,10 @@
       <c r="C45" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="3" t="s">
+      <c r="D45" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F45" s="0" t="s">
@@ -1955,10 +1998,10 @@
       <c r="C46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D46" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="0" t="s">
@@ -1981,10 +2024,10 @@
       <c r="C47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D47" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F47" s="0" t="s">
@@ -2007,10 +2050,10 @@
       <c r="C48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="D48" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F48" s="0" t="s">
@@ -2033,10 +2076,10 @@
       <c r="C49" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="D49" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F49" s="0" t="s">
@@ -2059,10 +2102,10 @@
       <c r="C50" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="D50" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F50" s="0" t="s">
@@ -2085,10 +2128,10 @@
       <c r="C51" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="D51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F51" s="0" t="s">
@@ -2111,10 +2154,10 @@
       <c r="C52" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="D52" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="0" t="s">
@@ -2137,10 +2180,10 @@
       <c r="C53" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="D53" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F53" s="0" t="s">
@@ -2163,10 +2206,10 @@
       <c r="C54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="D54" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F54" s="0" t="s">
@@ -2189,10 +2232,10 @@
       <c r="C55" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="D55" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F55" s="0" t="s">
@@ -2215,10 +2258,10 @@
       <c r="C56" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="D56" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F56" s="0" t="s">
@@ -2241,10 +2284,10 @@
       <c r="C57" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D57" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F57" s="0" t="s">
@@ -2267,10 +2310,10 @@
       <c r="C58" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="3" t="s">
+      <c r="D58" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F58" s="0" t="s">
@@ -2293,10 +2336,10 @@
       <c r="C59" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="D59" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F59" s="0" t="s">
@@ -2319,10 +2362,10 @@
       <c r="C60" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D60" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F60" s="0" t="s">
@@ -2345,10 +2388,10 @@
       <c r="C61" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="D61" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F61" s="0" t="s">
@@ -2371,10 +2414,10 @@
       <c r="C62" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="3" t="s">
+      <c r="D62" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F62" s="0" t="s">
@@ -2397,10 +2440,10 @@
       <c r="C63" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="D63" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F63" s="0" t="s">
@@ -2423,10 +2466,10 @@
       <c r="C64" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="D64" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F64" s="0" t="s">
@@ -2441,54 +2484,54 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>150</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="H66" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="G66" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,155 +2539,155 @@
         <v>45</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" s="3" t="s">
+      <c r="D67" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="H69" s="0" t="s">
         <v>163</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="G69" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="H69" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="H71" s="0" t="s">
         <v>168</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2652,77 +2695,77 @@
         <v>68</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G75" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="G75" s="0" t="s">
-        <v>170</v>
-      </c>
       <c r="H75" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,51 +2773,51 @@
         <v>68</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="H76" s="0" t="s">
         <v>173</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="G76" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H76" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="H77" s="0" t="s">
         <v>177</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="G77" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H77" s="0" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2782,25 +2825,25 @@
         <v>68</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,15 +2851,15 @@
         <v>68</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F79" s="0" t="s">
@@ -2834,25 +2877,25 @@
         <v>68</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2860,25 +2903,25 @@
         <v>68</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2886,25 +2929,25 @@
         <v>68</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" s="0" t="s">
+      <c r="G82" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="G82" s="0" t="s">
+      <c r="H82" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="H82" s="0" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,25 +2955,25 @@
         <v>68</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,25 +2981,25 @@
         <v>68</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" s="3" t="s">
+      <c r="D84" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,25 +3007,25 @@
         <v>68</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E85" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2990,25 +3033,25 @@
         <v>68</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="G86" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F86" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="G86" s="0" t="s">
-        <v>196</v>
-      </c>
       <c r="H86" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3016,66 +3059,160 @@
         <v>68</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C87" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="H87" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="G87" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="H87" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D89" s="4" t="n">
-        <f aca="false">COUNTIFS(D2:D87, "Yes")</f>
+      <c r="D89" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H89" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H90" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="H91" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C93" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D93" s="4" t="n">
+        <f aca="false">COUNTIFS(D2:D91, "Yes")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D90" s="4" t="n">
-        <f aca="false">COUNTIFS(D2:D87, "Maybe")</f>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D94" s="4" t="n">
+        <f aca="false">COUNTIFS(D2:D91, "Maybe")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D91" s="4" t="n">
-        <f aca="false">COUNTIFS(D2:D87, "No")</f>
-        <v>86</v>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" s="4" t="n">
+        <f aca="false">COUNTIFS(D2:D91, "No")</f>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H87"/>
-  <dataValidations count="2">
-    <dataValidation allowBlank="false" errorStyle="warning" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D87" type="list">
-      <formula1>"Yes,Maybe,No"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="warning" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E87" type="list">
-      <formula1>"Yes,No"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
+  <autoFilter ref="A1:H91"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
[season_calendar_spreadsheets] Add and update some 2022 concerts in CSV/XLSX
</commit_message>
<xml_diff>
--- a/season_calendar_spreadsheets/sso_2022_season_performances.xlsx
+++ b/season_calendar_spreadsheets/sso_2022_season_performances.xlsx
@@ -10,9 +10,6 @@
   <sheets>
     <sheet name="sso_2022_season_performances" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">sso_2022_season_performances!$A$1:$H$91</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="240">
   <si>
     <t xml:space="preserve">venue</t>
   </si>
@@ -109,7 +106,7 @@
     <t xml:space="preserve">Diana Doherty performs Strauss' Oboe Concerto</t>
   </si>
   <si>
-    <t xml:space="preserve">Written late in his life, Strauss’ Oboe Concerto is a dazzling masterclass in melody by one of the greatest of melodists, and its rich, flowing writing is skilfully brought to life by our Principal Oboe Diana Doherty. Known around the world for her prodigious talent and dynamic stage presence, her bravura performances of this work set her apart from all others. If you’ve never heard the extraordinarily expressive power of the oboe as a solo instrument, this is the perfect place to start.</t>
+    <t xml:space="preserve">Mendelssohn’s imagination was fired by the past. Standing in the ruins of Holyrood House in Edinburgh, he mused ‘Grass and ivy grow at the broken altar where Mary was crowned Queen of Scotland’. Here his Symphony No.3 begins, often referred to as the ScottishSymphony. It evokes the wild Romantic landscapes of Scotland and its rich past.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.sydneysymphony.com/concerts/diana-doherty-performs-strauss-oboe-concerto</t>
@@ -139,13 +136,43 @@
     <t xml:space="preserve">Sat 07 May</t>
   </si>
   <si>
+    <t xml:space="preserve">Newcastle City Hall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed 25 May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:30pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy &amp; Elation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felix Mendelssohn’s overture to Victor Hugo’s play Ruy Blas skilfully sets the stage for a dramatic and tragic tale, with a brooding opening that quickly finds its feet with an energetic melody, before sweeping into a spirited finale. It’s a curtain raiser that’s sure to delight. The mood continues with Haydn’s Trumpet Concerto. It’s a rare chance to hear a trumpet take the lead as a solo instrument, and just as rare to hear Sydney Symphony’s brilliant and renowned Principal Trumpet, David Elton, bring this unique composition to life.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sydneysymphony.com/concerts/energy-elation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamworth War Memorial Town Hall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu 26 May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Glasshouse, Port Macquarie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri 27 May</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wed 01 June</t>
   </si>
   <si>
     <t xml:space="preserve">Alexander Gavrylyuk performs Rachmaninov 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Rachmaninov’s Second Piano Concerto is not only one of his most famous pieces, but the work that truly established him as a composer of extraordinary power. With searing honesty in every emotion, Rachmaninov’s passion finds an exciting voice in soloist Alexander Gavrylyuk.</t>
+    <t xml:space="preserve">Prokofiev was, like Mozart, a child prodigy excelling in both piano and composition. At age 21 he created his first piano concerto, with a piano part that glitters and sparkles with a brilliant clarity. It’s a cheeky, playful piece with a trademark wit for which the which the mature Prokofiev became famous.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.sydneysymphony.com/concerts/alexander-gavrylyuk-performs-rachmaninov2</t>
@@ -193,6 +220,33 @@
     <t xml:space="preserve">Thu 09 June</t>
   </si>
   <si>
+    <t xml:space="preserve">Griffith Regional Theatre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed 15 June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Masters of Romance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Beethoven’s masterly Coriolan Overture, a relentless dramatic energy battles against a softer lyrical theme. Written to introduce a play about the Roman General Coriolanus, it’s a powerful depiction of the his emotional journey from ruthlessness to tenderness – and a perfect opening to this Sydney Symphony experience.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sydneysymphony.com/concerts/the-masters-of-romance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wagga Wagga Civic Theatre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu 16 June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Llewellyn Hall, Canberra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri 17 June</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wed 22 June</t>
   </si>
   <si>
@@ -229,6 +283,21 @@
     <t xml:space="preserve">Sat 25 June</t>
   </si>
   <si>
+    <t xml:space="preserve">Orange Civic Theatre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu 07 July</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sydney Symphony performs Tchaikovsky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not only do we have the chance to hear one of the most in demand bassoonists in the country, but two of them, performing together. Bringing to life music from Vienna’s golden past, the Orchestra’s very own Todd Gibson-Cornish and Matthew Wilkie showcase the bright, happy music that once floated out across Vienna’s cobbled streets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sydneysymphony.com/concerts/sydney-symphony-perform-tchaikovsky-2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">Concert Hall, Sydney Opera House</t>
   </si>
   <si>
@@ -454,6 +523,21 @@
     <t xml:space="preserve">https://www.sydneysymphony.com/concerts/andrea-lam-performs-mozart</t>
   </si>
   <si>
+    <t xml:space="preserve">Fri 07 October</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archie Roach &amp; the Sydney Symphony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For over 30 Years, Archie Roach has been one of Australia’s most vital and celebrated voices, delivering heartbreakingly beautiful and honest music and campaigning tirelessly for the rights and opportunities of Indigenous Australians. For the first time, he joins the Sydney Symphony Orchestra for an unmissable concert experience at the Sydney Opera House.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sydneysymphony.com/concerts/archie-roach-sydney-symphony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sat 08 October</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sun 09 October</t>
   </si>
   <si>
@@ -656,24 +740,17 @@
   </si>
   <si>
     <t xml:space="preserve">Sat 10 December</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maybe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -693,25 +770,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -756,24 +814,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -789,21 +835,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="0" topLeftCell="F87" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
-      <selection pane="topRight" activeCell="D93" activeCellId="0" sqref="D93"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -812,35 +852,35 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="183.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="74.99"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
@@ -848,10 +888,10 @@
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -874,10 +914,10 @@
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -900,10 +940,10 @@
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -926,10 +966,10 @@
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -952,10 +992,10 @@
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -978,10 +1018,10 @@
       <c r="A7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
@@ -1004,10 +1044,10 @@
       <c r="A8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -1030,10 +1070,10 @@
       <c r="A9" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -1056,10 +1096,10 @@
       <c r="A10" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
@@ -1082,10 +1122,10 @@
       <c r="A11" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -1108,10 +1148,10 @@
       <c r="A12" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -1134,10 +1174,10 @@
       <c r="A13" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="0" t="s">
@@ -1158,13 +1198,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>11</v>
@@ -1173,75 +1213,75 @@
         <v>11</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="H15" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="0" t="s">
@@ -1251,24 +1291,24 @@
         <v>11</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>11</v>
@@ -1277,50 +1317,50 @@
         <v>11</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>11</v>
@@ -1329,24 +1369,24 @@
         <v>11</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>47</v>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>11</v>
@@ -1355,24 +1395,24 @@
         <v>11</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>11</v>
@@ -1381,50 +1421,50 @@
         <v>11</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="G23" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>63</v>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>11</v>
@@ -1433,76 +1473,76 @@
         <v>11</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="G25" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="0" t="s">
+      <c r="H25" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="0" t="s">
+      <c r="G26" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>11</v>
@@ -1511,24 +1551,24 @@
         <v>11</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>11</v>
@@ -1537,24 +1577,24 @@
         <v>11</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>25</v>
+        <v>80</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>11</v>
@@ -1563,24 +1603,24 @@
         <v>11</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>16</v>
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>11</v>
@@ -1589,24 +1629,24 @@
         <v>11</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>10</v>
+        <v>87</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>11</v>
@@ -1615,23 +1655,23 @@
         <v>11</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="0" t="s">
@@ -1641,24 +1681,24 @@
         <v>11</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>11</v>
@@ -1667,24 +1707,24 @@
         <v>11</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>11</v>
@@ -1693,24 +1733,24 @@
         <v>11</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>25</v>
+        <v>92</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>11</v>
@@ -1719,23 +1759,23 @@
         <v>11</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D36" s="0" t="s">
@@ -1745,24 +1785,24 @@
         <v>11</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>11</v>
@@ -1771,23 +1811,23 @@
         <v>11</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="0" t="s">
@@ -1797,23 +1837,23 @@
         <v>11</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="0" t="s">
@@ -1823,24 +1863,24 @@
         <v>11</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>16</v>
+        <v>92</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>11</v>
@@ -1849,24 +1889,24 @@
         <v>11</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>11</v>
@@ -1875,24 +1915,24 @@
         <v>11</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>11</v>
@@ -1901,23 +1941,23 @@
         <v>11</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D43" s="0" t="s">
@@ -1927,24 +1967,24 @@
         <v>11</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>11</v>
@@ -1953,24 +1993,24 @@
         <v>11</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>11</v>
@@ -1979,24 +2019,24 @@
         <v>11</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>25</v>
+        <v>92</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>11</v>
@@ -2005,24 +2045,24 @@
         <v>11</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>11</v>
@@ -2031,24 +2071,24 @@
         <v>11</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>63</v>
+        <v>92</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>11</v>
@@ -2057,24 +2097,24 @@
         <v>11</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>63</v>
+        <v>92</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>11</v>
@@ -2083,24 +2123,24 @@
         <v>11</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>11</v>
@@ -2109,23 +2149,23 @@
         <v>11</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="0" t="s">
@@ -2135,24 +2175,24 @@
         <v>11</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>11</v>
@@ -2161,23 +2201,23 @@
         <v>11</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C53" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D53" s="0" t="s">
@@ -2187,24 +2227,24 @@
         <v>11</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>16</v>
+        <v>92</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>11</v>
@@ -2213,24 +2253,24 @@
         <v>11</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>47</v>
+        <v>80</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>11</v>
@@ -2239,24 +2279,24 @@
         <v>11</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>25</v>
+        <v>80</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>11</v>
@@ -2265,24 +2305,24 @@
         <v>11</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>11</v>
@@ -2291,24 +2331,24 @@
         <v>11</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>11</v>
@@ -2317,24 +2357,24 @@
         <v>11</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>11</v>
@@ -2343,24 +2383,24 @@
         <v>11</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>16</v>
+        <v>92</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>11</v>
@@ -2369,24 +2409,24 @@
         <v>11</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>25</v>
+        <v>92</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>11</v>
@@ -2395,24 +2435,24 @@
         <v>11</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>11</v>
@@ -2421,24 +2461,24 @@
         <v>11</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>11</v>
@@ -2447,23 +2487,23 @@
         <v>11</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C64" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="0" t="s">
@@ -2473,24 +2513,24 @@
         <v>11</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>151</v>
+        <v>92</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>11</v>
@@ -2499,24 +2539,24 @@
         <v>11</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>155</v>
+        <v>92</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>11</v>
@@ -2525,24 +2565,24 @@
         <v>11</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>11</v>
@@ -2551,24 +2591,24 @@
         <v>11</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>11</v>
@@ -2577,24 +2617,24 @@
         <v>11</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>11</v>
@@ -2603,50 +2643,50 @@
         <v>11</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B70" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G70" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" s="0" t="s">
+      <c r="H70" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="G70" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="H70" s="0" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>63</v>
+        <v>92</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>11</v>
@@ -2655,24 +2695,24 @@
         <v>11</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>16</v>
+        <v>92</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>11</v>
@@ -2681,50 +2721,50 @@
         <v>11</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B73" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" s="0" t="s">
-        <v>171</v>
-      </c>
       <c r="G73" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>63</v>
+        <v>92</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>11</v>
@@ -2733,24 +2773,24 @@
         <v>11</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>11</v>
@@ -2759,24 +2799,24 @@
         <v>11</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>11</v>
@@ -2785,24 +2825,24 @@
         <v>11</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>11</v>
@@ -2811,24 +2851,24 @@
         <v>11</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>11</v>
@@ -2837,24 +2877,24 @@
         <v>11</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>47</v>
+        <v>80</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>11</v>
@@ -2863,24 +2903,24 @@
         <v>11</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>10</v>
+        <v>80</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>11</v>
@@ -2889,24 +2929,24 @@
         <v>11</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>11</v>
@@ -2915,24 +2955,24 @@
         <v>11</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>11</v>
@@ -2941,24 +2981,24 @@
         <v>11</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>16</v>
+        <v>80</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>11</v>
@@ -2967,24 +3007,24 @@
         <v>11</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>11</v>
@@ -2993,24 +3033,24 @@
         <v>11</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>11</v>
@@ -3019,24 +3059,24 @@
         <v>11</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>25</v>
+        <v>80</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>11</v>
@@ -3045,24 +3085,24 @@
         <v>11</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>11</v>
@@ -3071,24 +3111,24 @@
         <v>11</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>11</v>
@@ -3097,23 +3137,23 @@
         <v>11</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C89" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D89" s="0" t="s">
@@ -3123,23 +3163,23 @@
         <v>11</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C90" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D90" s="0" t="s">
@@ -3149,23 +3189,23 @@
         <v>11</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C91" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D91" s="0" t="s">
@@ -3175,44 +3215,250 @@
         <v>11</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>208</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="H92" s="0" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D93" s="4" t="n">
-        <f aca="false">COUNTIFS(D2:D91, "Yes")</f>
-        <v>0</v>
+      <c r="A93" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="H93" s="0" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D94" s="4" t="n">
-        <f aca="false">COUNTIFS(D2:D91, "Maybe")</f>
-        <v>0</v>
+      <c r="A94" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="H94" s="0" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="4" t="n">
-        <f aca="false">COUNTIFS(D2:D91, "No")</f>
-        <v>90</v>
+      <c r="A95" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="H95" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="G96" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="H97" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="G98" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="H98" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="H99" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="G100" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="H100" s="0" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H91"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3220,6 +3466,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>